<commit_message>
code2reqs should not postprocess reqs if used for tracing (#80)
* code2reqs should not postprocess reqs if used for tracing

* updating traceability expected results, need a proper test for this in deployment
</commit_message>
<xml_diff>
--- a/tests/test_outputs/test_csv_to_excel_with_traceability/csv_to_excel_with_traceability.xlsx
+++ b/tests/test_outputs/test_csv_to_excel_with_traceability/csv_to_excel_with_traceability.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Requirements" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Requirements" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -435,7 +435,7 @@
     <col width="20" customWidth="1" min="3" max="3"/>
     <col width="50" customWidth="1" min="4" max="4"/>
     <col width="7" customWidth="1" min="5" max="5"/>
-    <col width="11" customWidth="1" min="6" max="6"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
     <col width="5" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
@@ -565,7 +565,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Clear_Table</t>
+          <t>Add_Included_Dessert</t>
         </is>
       </c>
       <c r="G4" t="inlineStr"/>

</xml_diff>